<commit_message>
integration de l'unité de mesure dans l'importation des articles
</commit_message>
<xml_diff>
--- a/public/model.xlsx
+++ b/public/model.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>ABATTANT GOLF  A VALISETTE (2003 BP)</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>SANITAIRE ET PLOMBERIE</t>
+  </si>
+  <si>
+    <t>Unite</t>
   </si>
 </sst>
 </file>
@@ -451,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1763"/>
+  <dimension ref="A1:K1763"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -469,7 +472,7 @@
     <col min="10" max="10" width="23.6328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="7" customFormat="1">
+    <row r="1" spans="1:11" s="7" customFormat="1">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -500,8 +503,11 @@
       <c r="J1" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" s="14" customFormat="1">
+      <c r="K1" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="14" customFormat="1">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
@@ -524,99 +530,102 @@
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="K2" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="2"/>
       <c r="C3" s="8"/>
       <c r="D3" s="4"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:11">
       <c r="A4" s="2"/>
       <c r="C4" s="8"/>
       <c r="D4" s="4"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:11">
       <c r="A5" s="2"/>
       <c r="C5" s="8"/>
       <c r="D5" s="4"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:11">
       <c r="A6" s="2"/>
       <c r="C6" s="8"/>
       <c r="D6" s="4"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:11">
       <c r="A7" s="2"/>
       <c r="C7" s="8"/>
       <c r="D7" s="4"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:11">
       <c r="A8" s="2"/>
       <c r="C8" s="8"/>
       <c r="D8" s="4"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:11">
       <c r="A9" s="2"/>
       <c r="C9" s="8"/>
       <c r="D9" s="4"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:11">
       <c r="A10" s="2"/>
       <c r="C10" s="8"/>
       <c r="D10" s="4"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:11">
       <c r="A11" s="2"/>
       <c r="C11" s="8"/>
       <c r="D11" s="4"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:11">
       <c r="A12" s="2"/>
       <c r="C12" s="8"/>
       <c r="D12" s="4"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:11">
       <c r="A13" s="2"/>
       <c r="C13" s="8"/>
       <c r="D13" s="4"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:11">
       <c r="A14" s="2"/>
       <c r="C14" s="8"/>
       <c r="D14" s="4"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:11">
       <c r="A15" s="2"/>
       <c r="C15" s="8"/>
       <c r="D15" s="4"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:11">
       <c r="A16" s="2"/>
       <c r="C16" s="8"/>
       <c r="D16" s="4"/>

</xml_diff>